<commit_message>
accuracy predicted after training model
</commit_message>
<xml_diff>
--- a/dataset1.xlsx
+++ b/dataset1.xlsx
@@ -280,8 +280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B243" sqref="B243"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198:B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -297,2473 +297,2473 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">RAND() * (4 - 1) + 1</f>
-        <v>2.7592344023598794</v>
+        <v>3.5553621901365395</v>
       </c>
       <c r="B2">
         <f ca="1">A2*10</f>
-        <v>27.592344023598795</v>
+        <v>35.553621901365396</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A66" ca="1" si="0">RAND() * (4 - 1) + 1</f>
-        <v>2.4331011918354974</v>
+        <v>2.9502690605861424</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="1">A3*10</f>
-        <v>24.331011918354974</v>
+        <v>29.502690605861424</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2414399200746473</v>
+        <v>2.9084207154084663</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>32.414399200746473</v>
+        <v>29.084207154084663</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8060113042196626</v>
+        <v>1.3259879600635767</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>28.060113042196626</v>
+        <v>13.259879600635767</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3368184438061914</v>
+        <v>1.492818997057257</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>23.368184438061913</v>
+        <v>14.92818997057257</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8578346923608873</v>
+        <v>1.0840437473700963</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>38.578346923608876</v>
+        <v>10.840437473700963</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6505985963569438</v>
+        <v>3.0226083056779958</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>36.505985963569437</v>
+        <v>30.226083056779956</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6268791022634654</v>
+        <v>3.6020023095373679</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>16.268791022634655</v>
+        <v>36.020023095373681</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9588300739161899</v>
+        <v>1.4923689044379249</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>29.588300739161898</v>
+        <v>14.923689044379248</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3337111834238349</v>
+        <v>2.1934109919242983</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>23.33711183423835</v>
+        <v>21.934109919242985</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0498315376225928</v>
+        <v>2.0293365952290956</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>30.498315376225928</v>
+        <v>20.293365952290955</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5017101566625786</v>
+        <v>3.6458700385986629</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>25.017101566625787</v>
+        <v>36.458700385986631</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6766439001237476</v>
+        <v>3.3672980574314328</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>16.766439001237476</v>
+        <v>33.67298057431433</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5897912313026823</v>
+        <v>2.2440604146534588</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>25.897912313026822</v>
+        <v>22.440604146534589</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4448623596069092</v>
+        <v>1.0877407807427257</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>14.448623596069092</v>
+        <v>10.877407807427257</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5309093964096467</v>
+        <v>2.1285794536152518</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>25.309093964096469</v>
+        <v>21.285794536152519</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3814037976633626</v>
+        <v>1.2175371333172591</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>23.814037976633628</v>
+        <v>12.175371333172592</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9592919913997409</v>
+        <v>1.7024491010617782</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>39.592919913997406</v>
+        <v>17.02449101061778</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3588888231225744</v>
+        <v>3.8537653542642634</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>33.588888231225745</v>
+        <v>38.53765354264263</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4365372052648868</v>
+        <v>3.7212625068090195</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>14.365372052648869</v>
+        <v>37.212625068090198</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8668378756685584</v>
+        <v>3.2892581500250477</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>38.668378756685584</v>
+        <v>32.892581500250479</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3545397110658741</v>
+        <v>1.9578248059057999</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>23.54539711065874</v>
+        <v>19.578248059057998</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1647459788758807</v>
+        <v>1.8369037536557207</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.647459788758807</v>
+        <v>18.369037536557208</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8342006474324228</v>
+        <v>1.6188199754077037</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>18.342006474324229</v>
+        <v>16.188199754077036</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7793507895953642</v>
+        <v>2.8897115225834975</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>17.793507895953642</v>
+        <v>28.897115225834973</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9036780291442337</v>
+        <v>3.1832195557443956</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>19.036780291442337</v>
+        <v>31.832195557443956</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6039124666593518</v>
+        <v>3.8457070030162788</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>36.039124666593516</v>
+        <v>38.457070030162789</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2652684002957244</v>
+        <v>2.9609463221648626</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>22.652684002957244</v>
+        <v>29.609463221648625</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9423934773038694</v>
+        <v>1.5350714371276217</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>29.423934773038695</v>
+        <v>15.350714371276217</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9601197056669344</v>
+        <v>2.7677941969540356</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>19.601197056669342</v>
+        <v>27.677941969540356</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1039381544584659</v>
+        <v>1.3568758015722495</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>31.039381544584657</v>
+        <v>13.568758015722494</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>2.087882006081986</v>
+        <v>1.7219743319508987</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>20.878820060819862</v>
+        <v>17.219743319508986</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8342355380548852</v>
+        <v>1.4246711003853965</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>38.342355380548852</v>
+        <v>14.246711003853964</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2750525662968872</v>
+        <v>3.8369474735553042</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>22.750525662968872</v>
+        <v>38.369474735553041</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9051377997287355</v>
+        <v>1.0217060820362669</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>39.051377997287354</v>
+        <v>10.217060820362668</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5778312778871786</v>
+        <v>2.4760976128771626</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>15.778312778871786</v>
+        <v>24.760976128771624</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0617459083163574</v>
+        <v>2.5660740280501537</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>20.617459083163574</v>
+        <v>25.660740280501535</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5292784212643658</v>
+        <v>3.0500901755574077</v>
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>25.292784212643657</v>
+        <v>30.500901755574077</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7324223789630016</v>
+        <v>2.0818186798622853</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>17.324223789630015</v>
+        <v>20.818186798622854</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4434591056003643</v>
+        <v>3.4038730563918209</v>
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>34.43459105600364</v>
+        <v>34.038730563918207</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1728564308803944</v>
+        <v>2.2561247523128793</v>
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>21.728564308803943</v>
+        <v>22.561247523128792</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3130681128568322</v>
+        <v>2.1232136059848594</v>
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>33.13068112856832</v>
+        <v>21.232136059848592</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2537785206021166</v>
+        <v>1.7970727987467063</v>
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>22.537785206021166</v>
+        <v>17.970727987467065</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4366175586100454</v>
+        <v>3.9041538944471359</v>
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>24.366175586100454</v>
+        <v>39.041538944471355</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4783362164939051</v>
+        <v>2.37626945553873</v>
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>34.783362164939049</v>
+        <v>23.762694555387299</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1560447484899892</v>
+        <v>1.9087072022931144</v>
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>11.560447484899893</v>
+        <v>19.087072022931146</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7768327239808772</v>
+        <v>1.3580072629429563</v>
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>37.768327239808769</v>
+        <v>13.580072629429562</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5958162074457163</v>
+        <v>3.4782392385094565</v>
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>25.958162074457164</v>
+        <v>34.782392385094568</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1647291001986724</v>
+        <v>2.5013645620573159</v>
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>21.647291001986723</v>
+        <v>25.013645620573158</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2625587351126073</v>
+        <v>3.531797123345449</v>
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>12.625587351126073</v>
+        <v>35.317971233454493</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8702984782778542</v>
+        <v>3.5336316562041814</v>
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>38.702984782778543</v>
+        <v>35.336316562041816</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>1.899012048343137</v>
+        <v>1.1083836084860814</v>
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>18.990120483431369</v>
+        <v>11.083836084860813</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7147407372125523</v>
+        <v>1.6444995892830514</v>
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>17.147407372125521</v>
+        <v>16.444995892830512</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9288943057149743</v>
+        <v>2.7563080880283701</v>
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>39.288943057149744</v>
+        <v>27.5630808802837</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7489694743355901</v>
+        <v>3.7860700330543735</v>
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>37.489694743355898</v>
+        <v>37.860700330543736</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3595458241338543</v>
+        <v>1.1913940125229532</v>
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>33.595458241338541</v>
+        <v>11.913940125229532</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5726912457941888</v>
+        <v>2.1120496462372489</v>
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>25.726912457941889</v>
+        <v>21.12049646237249</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6102095614735785</v>
+        <v>2.3919923623473225</v>
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>16.102095614735784</v>
+        <v>23.919923623473224</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2163472721585906</v>
+        <v>3.3897553728864125</v>
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>32.163472721585904</v>
+        <v>33.897553728864125</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2768140290534342</v>
+        <v>1.2665582256438404</v>
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>12.768140290534342</v>
+        <v>12.665582256438404</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8416593659440568</v>
+        <v>3.6912054423379113</v>
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>18.416593659440569</v>
+        <v>36.912054423379111</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9318839906935223</v>
+        <v>3.4235063241295398</v>
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>29.318839906935224</v>
+        <v>34.2350632412954</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7802239773228372</v>
+        <v>3.1620336088202956</v>
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>27.802239773228372</v>
+        <v>31.620336088202954</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3442101225901983</v>
+        <v>3.2453528677104346</v>
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>13.442101225901983</v>
+        <v>32.453528677104345</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5193761994248147</v>
+        <v>2.351323985984398</v>
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>25.193761994248149</v>
+        <v>23.513239859843978</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" ref="A67:A130" ca="1" si="2">RAND() * (4 - 1) + 1</f>
-        <v>3.9558062182124849</v>
+        <v>1.1841565870951012</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" ca="1" si="3">A67*10</f>
-        <v>39.55806218212485</v>
+        <v>11.841565870951012</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5088861680349339</v>
+        <v>1.9620456487423032</v>
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="3"/>
-        <v>35.088861680349339</v>
+        <v>19.620456487423034</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1757866132351347</v>
+        <v>1.477657415311703</v>
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="3"/>
-        <v>31.757866132351346</v>
+        <v>14.77657415311703</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5598200737678602</v>
+        <v>3.7739175882881613</v>
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="3"/>
-        <v>15.598200737678603</v>
+        <v>37.739175882881611</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7468771113490031</v>
+        <v>3.7586662245218267</v>
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="3"/>
-        <v>17.468771113490032</v>
+        <v>37.586662245218264</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0383049085224922</v>
+        <v>1.6510539661672761</v>
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="3"/>
-        <v>10.383049085224922</v>
+        <v>16.510539661672759</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9820802199808081</v>
+        <v>2.9889445050690195</v>
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="3"/>
-        <v>39.820802199808078</v>
+        <v>29.889445050690195</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0181685291117679</v>
+        <v>1.027942724690984</v>
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="3"/>
-        <v>10.181685291117679</v>
+        <v>10.27942724690984</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9954099016225448</v>
+        <v>3.8664318448025341</v>
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="3"/>
-        <v>19.954099016225449</v>
+        <v>38.664318448025341</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1064418480284708</v>
+        <v>1.8685248493058961</v>
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="3"/>
-        <v>31.064418480284708</v>
+        <v>18.68524849305896</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1136753235776728</v>
+        <v>1.8275680069818163</v>
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="3"/>
-        <v>11.136753235776728</v>
+        <v>18.275680069818165</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1868796354320779</v>
+        <v>2.7087420500688122</v>
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="3"/>
-        <v>31.868796354320779</v>
+        <v>27.087420500688122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4623750204612396</v>
+        <v>3.7189171355263846</v>
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="3"/>
-        <v>34.623750204612392</v>
+        <v>37.189171355263845</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" ca="1" si="2"/>
-        <v>2.108404223326442</v>
+        <v>2.6942234042441315</v>
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="3"/>
-        <v>21.08404223326442</v>
+        <v>26.942234042441314</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7341778938141297</v>
+        <v>2.1469045508021134</v>
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="3"/>
-        <v>17.341778938141296</v>
+        <v>21.469045508021132</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4779799487241776</v>
+        <v>3.7054019853241726</v>
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="3"/>
-        <v>14.779799487241776</v>
+        <v>37.054019853241726</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4621194410939533</v>
+        <v>2.2628140218472184</v>
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="3"/>
-        <v>34.62119441093953</v>
+        <v>22.628140218472183</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4473854218924398</v>
+        <v>1.4265111990346395</v>
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="3"/>
-        <v>24.473854218924398</v>
+        <v>14.265111990346394</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3349852545733425</v>
+        <v>2.052393826714868</v>
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="3"/>
-        <v>13.349852545733425</v>
+        <v>20.523938267148679</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" ca="1" si="2"/>
-        <v>3.539025786870885</v>
+        <v>2.1093903171571071</v>
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="3"/>
-        <v>35.390257868708851</v>
+        <v>21.093903171571071</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5057362860546406</v>
+        <v>1.504206939567591</v>
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="3"/>
-        <v>25.057362860546405</v>
+        <v>15.04206939567591</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5416758335324836</v>
+        <v>3.9128694514181066</v>
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="3"/>
-        <v>15.416758335324836</v>
+        <v>39.128694514181063</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0024776585736785</v>
+        <v>1.4259867668751047</v>
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="3"/>
-        <v>30.024776585736785</v>
+        <v>14.259867668751047</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4270204983913217</v>
+        <v>1.2745839046969962</v>
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="3"/>
-        <v>34.270204983913217</v>
+        <v>12.745839046969962</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" ca="1" si="2"/>
-        <v>2.439787171595726</v>
+        <v>2.9833082506090181</v>
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="3"/>
-        <v>24.397871715957258</v>
+        <v>29.833082506090179</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6953216543135712</v>
+        <v>2.2928890224829073</v>
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="3"/>
-        <v>26.95321654313571</v>
+        <v>22.928890224829072</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6935467208665589</v>
+        <v>3.7578140889261804</v>
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="3"/>
-        <v>26.935467208665589</v>
+        <v>37.578140889261803</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4855226878046932</v>
+        <v>3.5929870915335442</v>
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="3"/>
-        <v>24.855226878046931</v>
+        <v>35.929870915335442</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0780813263717772</v>
+        <v>1.0944552209894001</v>
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="3"/>
-        <v>20.780813263717771</v>
+        <v>10.944552209894001</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7380532697171289</v>
+        <v>3.612880832390279</v>
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="3"/>
-        <v>17.38053269717129</v>
+        <v>36.128808323902788</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" ca="1" si="2"/>
-        <v>2.245770706456482</v>
+        <v>1.8391288160220767</v>
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="3"/>
-        <v>22.457707064564822</v>
+        <v>18.391288160220768</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1706173884793025</v>
+        <v>3.0098812227766767</v>
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="3"/>
-        <v>11.706173884793024</v>
+        <v>30.098812227766768</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8213670007782392</v>
+        <v>1.9394419800263059</v>
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="3"/>
-        <v>28.21367000778239</v>
+        <v>19.394419800263059</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2747267928324675</v>
+        <v>2.6519793084672258</v>
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="3"/>
-        <v>22.747267928324675</v>
+        <v>26.519793084672258</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4429985339246421</v>
+        <v>2.5164915921387712</v>
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="3"/>
-        <v>14.429985339246421</v>
+        <v>25.16491592138771</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7434636817622202</v>
+        <v>3.9385203521816718</v>
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="3"/>
-        <v>17.434636817622202</v>
+        <v>39.38520352181672</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5003462641484524</v>
+        <v>1.515453431362122</v>
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="3"/>
-        <v>15.003462641484525</v>
+        <v>15.15453431362122</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8596175680271454</v>
+        <v>3.9257435614575531</v>
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="3"/>
-        <v>38.596175680271458</v>
+        <v>39.257435614575527</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" ca="1" si="2"/>
-        <v>1.8142403243870686</v>
+        <v>1.5866808171843356</v>
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="3"/>
-        <v>18.142403243870685</v>
+        <v>15.866808171843356</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3372903736960113</v>
+        <v>1.4260622985105327</v>
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="3"/>
-        <v>33.372903736960112</v>
+        <v>14.260622985105327</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7001129298553259</v>
+        <v>1.1856260697360552</v>
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="3"/>
-        <v>37.001129298553259</v>
+        <v>11.856260697360552</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" ca="1" si="2"/>
-        <v>1.8011211043575051</v>
+        <v>3.438185777544418</v>
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="3"/>
-        <v>18.011211043575052</v>
+        <v>34.381857775444182</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5261867613318771</v>
+        <v>3.5833466342425861</v>
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="3"/>
-        <v>25.261867613318771</v>
+        <v>35.833466342425865</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0062549873102924</v>
+        <v>2.0130677960686532</v>
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="3"/>
-        <v>20.062549873102924</v>
+        <v>20.130677960686533</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6135083982667684</v>
+        <v>3.922760965097924</v>
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="3"/>
-        <v>26.135083982667684</v>
+        <v>39.22760965097924</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" ca="1" si="2"/>
-        <v>1.8654702843538518</v>
+        <v>2.7964461973344408</v>
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="3"/>
-        <v>18.654702843538516</v>
+        <v>27.964461973344406</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3804401368045598</v>
+        <v>2.4363695493120319</v>
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="3"/>
-        <v>33.804401368045596</v>
+        <v>24.363695493120318</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1700967545329406</v>
+        <v>1.5050918048114785</v>
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="3"/>
-        <v>11.700967545329405</v>
+        <v>15.050918048114784</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7451045130956211</v>
+        <v>2.6146500626160529</v>
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="3"/>
-        <v>27.45104513095621</v>
+        <v>26.146500626160531</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5530759816640762</v>
+        <v>3.1953455027712785</v>
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="3"/>
-        <v>15.530759816640762</v>
+        <v>31.953455027712785</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5510982221594705</v>
+        <v>2.5186682127001601</v>
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="3"/>
-        <v>15.510982221594706</v>
+        <v>25.1866821270016</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" ca="1" si="2"/>
-        <v>3.170757015956331</v>
+        <v>1.9190780267801271</v>
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="3"/>
-        <v>31.707570159563311</v>
+        <v>19.190780267801269</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9663657766347344</v>
+        <v>2.0267640743343156</v>
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="3"/>
-        <v>29.663657766347345</v>
+        <v>20.267640743343158</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5499867297768177</v>
+        <v>3.0470092966374218</v>
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="3"/>
-        <v>25.499867297768176</v>
+        <v>30.470092966374217</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" ca="1" si="2"/>
-        <v>1.852004954846076</v>
+        <v>1.5256792082817516</v>
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="3"/>
-        <v>18.520049548460761</v>
+        <v>15.256792082817515</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0855759396513984</v>
+        <v>3.7117068729368987</v>
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="3"/>
-        <v>30.855759396513985</v>
+        <v>37.117068729368988</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9933517798050175</v>
+        <v>2.0568789121128779</v>
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="3"/>
-        <v>19.933517798050175</v>
+        <v>20.568789121128781</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" ca="1" si="2"/>
-        <v>3.2731144110412647</v>
+        <v>2.2240678245202581</v>
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="3"/>
-        <v>32.731144110412643</v>
+        <v>22.240678245202581</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" ca="1" si="2"/>
-        <v>2.1859190100099526</v>
+        <v>1.9251320784887636</v>
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="3"/>
-        <v>21.859190100099525</v>
+        <v>19.251320784887636</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0686442002613346</v>
+        <v>1.3907825710105286</v>
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="3"/>
-        <v>10.686442002613346</v>
+        <v>13.907825710105286</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3155300184796728</v>
+        <v>2.0426935278606053</v>
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="3"/>
-        <v>33.155300184796729</v>
+        <v>20.426935278606052</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4517297114842993</v>
+        <v>1.0916754901663366</v>
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="3"/>
-        <v>14.517297114842993</v>
+        <v>10.916754901663365</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6692828834099782</v>
+        <v>1.7425075237419749</v>
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="3"/>
-        <v>16.692828834099782</v>
+        <v>17.425075237419748</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" ca="1" si="2"/>
-        <v>3.2738927726061826</v>
+        <v>2.412393272621626</v>
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="3"/>
-        <v>32.738927726061824</v>
+        <v>24.12393272621626</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" ref="A131:A194" ca="1" si="4">RAND() * (4 - 1) + 1</f>
-        <v>1.5561137984747782</v>
+        <v>1.1408532868914003</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B194" ca="1" si="5">A131*10</f>
-        <v>15.561137984747781</v>
+        <v>11.408532868914003</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ca="1" si="4"/>
-        <v>2.5654219902791988</v>
+        <v>3.7685933417757318</v>
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="5"/>
-        <v>25.654219902791986</v>
+        <v>37.685933417757319</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" ca="1" si="4"/>
-        <v>3.1242619873037758</v>
+        <v>2.1290032342311487</v>
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="5"/>
-        <v>31.242619873037757</v>
+        <v>21.290032342311488</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4832975450159225</v>
+        <v>1.1942737623422668</v>
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="5"/>
-        <v>24.832975450159225</v>
+        <v>11.942737623422667</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8020604146037291</v>
+        <v>1.9109343822471629</v>
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="5"/>
-        <v>28.020604146037293</v>
+        <v>19.109343822471629</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1263375453476732</v>
+        <v>2.6198703699853874</v>
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="5"/>
-        <v>21.263375453476733</v>
+        <v>26.198703699853873</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2837626434984453</v>
+        <v>2.7631033650811547</v>
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="5"/>
-        <v>12.837626434984452</v>
+        <v>27.631033650811545</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4133025453886736</v>
+        <v>2.9396082775866401</v>
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="5"/>
-        <v>14.133025453886736</v>
+        <v>29.3960827758664</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3661608753681338</v>
+        <v>2.8055542808355671</v>
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="5"/>
-        <v>23.661608753681339</v>
+        <v>28.055542808355671</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" ca="1" si="4"/>
-        <v>3.6017381830602604</v>
+        <v>1.1861088747993249</v>
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="5"/>
-        <v>36.017381830602602</v>
+        <v>11.86108874799325</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3923747316685571</v>
+        <v>2.9422927121068714</v>
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="5"/>
-        <v>23.923747316685571</v>
+        <v>29.422927121068714</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1870223972210594</v>
+        <v>1.2576515882878725</v>
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="5"/>
-        <v>21.870223972210596</v>
+        <v>12.576515882878725</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8019756504189548</v>
+        <v>1.6138884219095819</v>
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="5"/>
-        <v>28.019756504189548</v>
+        <v>16.138884219095818</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" ca="1" si="4"/>
-        <v>2.5265803297604474</v>
+        <v>3.0946004535201532</v>
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="5"/>
-        <v>25.265803297604474</v>
+        <v>30.946004535201531</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0320352534753381</v>
+        <v>3.722548363459131</v>
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="5"/>
-        <v>10.320352534753381</v>
+        <v>37.225483634591313</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8817402282617564</v>
+        <v>2.3961845350938584</v>
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="5"/>
-        <v>28.817402282617564</v>
+        <v>23.961845350938585</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" ca="1" si="4"/>
-        <v>3.2086193763677384</v>
+        <v>1.1668140763458086</v>
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="5"/>
-        <v>32.086193763677386</v>
+        <v>11.668140763458085</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5577738059187838</v>
+        <v>3.5251312292809347</v>
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="5"/>
-        <v>15.577738059187837</v>
+        <v>35.251312292809345</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" ca="1" si="4"/>
-        <v>3.7136297254889077</v>
+        <v>1.653549684510156</v>
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="5"/>
-        <v>37.13629725488908</v>
+        <v>16.535496845101562</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" ca="1" si="4"/>
-        <v>1.481360975949719</v>
+        <v>3.6226872406300461</v>
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="5"/>
-        <v>14.81360975949719</v>
+        <v>36.226872406300458</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" ca="1" si="4"/>
-        <v>3.2022673542645421</v>
+        <v>3.789760178649511</v>
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="5"/>
-        <v>32.022673542645421</v>
+        <v>37.897601786495109</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" ca="1" si="4"/>
-        <v>3.2960658377955632</v>
+        <v>1.7857825758980206</v>
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="5"/>
-        <v>32.960658377955632</v>
+        <v>17.857825758980205</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9446256058358689</v>
+        <v>2.6466118564607619</v>
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="5"/>
-        <v>29.446256058358689</v>
+        <v>26.466118564607619</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9213473139818253</v>
+        <v>3.7243650240403925</v>
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="5"/>
-        <v>19.213473139818255</v>
+        <v>37.243650240403923</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9902151526771719</v>
+        <v>1.5307481345078529</v>
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="5"/>
-        <v>19.902151526771718</v>
+        <v>15.307481345078529</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5514769640668864</v>
+        <v>3.0408107524460322</v>
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="5"/>
-        <v>35.514769640668867</v>
+        <v>30.40810752446032</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" ca="1" si="4"/>
-        <v>3.0851444700391459</v>
+        <v>1.8661991119175441</v>
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="5"/>
-        <v>30.851444700391461</v>
+        <v>18.66199111917544</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2064910271746889</v>
+        <v>1.4639994851610874</v>
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="5"/>
-        <v>12.064910271746889</v>
+        <v>14.639994851610874</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9862822430638181</v>
+        <v>3.9607177765694384</v>
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="5"/>
-        <v>19.862822430638182</v>
+        <v>39.607177765694381</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9210107077642604</v>
+        <v>3.1431987478746506</v>
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="5"/>
-        <v>19.210107077642604</v>
+        <v>31.431987478746507</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0045753024059501</v>
+        <v>1.4352065813662502</v>
       </c>
       <c r="B161">
         <f t="shared" ca="1" si="5"/>
-        <v>20.045753024059501</v>
+        <v>14.352065813662502</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" ca="1" si="4"/>
-        <v>3.3913340175975915</v>
+        <v>3.6259093132285272</v>
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="5"/>
-        <v>33.913340175975918</v>
+        <v>36.259093132285273</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1448274213250293</v>
+        <v>3.4928727609300281</v>
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="5"/>
-        <v>21.448274213250293</v>
+        <v>34.928727609300282</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2100331384950422</v>
+        <v>1.1072058897159971</v>
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="5"/>
-        <v>12.100331384950422</v>
+        <v>11.072058897159971</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3954105506891716</v>
+        <v>3.6469053562797882</v>
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="5"/>
-        <v>23.954105506891715</v>
+        <v>36.469053562797882</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5247052279211708</v>
+        <v>3.5005055000177108</v>
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="5"/>
-        <v>15.247052279211708</v>
+        <v>35.005055000177109</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7172525406056636</v>
+        <v>3.9830600829997982</v>
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="5"/>
-        <v>27.172525406056636</v>
+        <v>39.830600829997984</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
         <f t="shared" ca="1" si="4"/>
-        <v>3.280148030275547</v>
+        <v>2.0973180899952371</v>
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="5"/>
-        <v>32.801480302755472</v>
+        <v>20.973180899952371</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
         <f t="shared" ca="1" si="4"/>
-        <v>3.7670056737842583</v>
+        <v>1.5912346381943347</v>
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="5"/>
-        <v>37.670056737842586</v>
+        <v>15.912346381943347</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8782907768490364</v>
+        <v>1.4205418413306492</v>
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="5"/>
-        <v>28.782907768490364</v>
+        <v>14.205418413306493</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
         <f t="shared" ca="1" si="4"/>
-        <v>2.291377066624352</v>
+        <v>2.044418014869533</v>
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="5"/>
-        <v>22.913770666243522</v>
+        <v>20.444180148695331</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
         <f t="shared" ca="1" si="4"/>
-        <v>3.913777224564801</v>
+        <v>3.7990370701784775</v>
       </c>
       <c r="B172">
         <f t="shared" ca="1" si="5"/>
-        <v>39.137772245648009</v>
+        <v>37.990370701784776</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173">
         <f t="shared" ca="1" si="4"/>
-        <v>2.5874353357536934</v>
+        <v>1.6407299040756871</v>
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="5"/>
-        <v>25.874353357536933</v>
+        <v>16.407299040756872</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174">
         <f t="shared" ca="1" si="4"/>
-        <v>2.5518373092830924</v>
+        <v>2.6578067209313918</v>
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="5"/>
-        <v>25.518373092830924</v>
+        <v>26.578067209313918</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5640216327888146</v>
+        <v>1.7715908700576311</v>
       </c>
       <c r="B175">
         <f t="shared" ca="1" si="5"/>
-        <v>35.640216327888147</v>
+        <v>17.715908700576311</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4800242795099363</v>
+        <v>3.7769153469035803</v>
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="5"/>
-        <v>34.800242795099365</v>
+        <v>37.7691534690358</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2585357340028629</v>
+        <v>3.0423395314205406</v>
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="5"/>
-        <v>12.585357340028629</v>
+        <v>30.423395314205408</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7969880574610517</v>
+        <v>3.6580340474257738</v>
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="5"/>
-        <v>27.969880574610517</v>
+        <v>36.580340474257738</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179">
         <f t="shared" ca="1" si="4"/>
-        <v>3.9702305153695319</v>
+        <v>1.0504791103236708</v>
       </c>
       <c r="B179">
         <f t="shared" ca="1" si="5"/>
-        <v>39.70230515369532</v>
+        <v>10.504791103236709</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180">
         <f t="shared" ca="1" si="4"/>
-        <v>3.1921084702902687</v>
+        <v>2.6006029372246195</v>
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="5"/>
-        <v>31.921084702902686</v>
+        <v>26.006029372246196</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3942145995596027</v>
+        <v>2.596771836828347</v>
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="5"/>
-        <v>23.942145995596029</v>
+        <v>25.967718368283471</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182">
         <f t="shared" ca="1" si="4"/>
-        <v>2.549332099946692</v>
+        <v>2.807689042536448</v>
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="5"/>
-        <v>25.493320999466921</v>
+        <v>28.076890425364482</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183">
         <f t="shared" ca="1" si="4"/>
-        <v>3.0190325118598804</v>
+        <v>2.5848368860948878</v>
       </c>
       <c r="B183">
         <f t="shared" ca="1" si="5"/>
-        <v>30.190325118598803</v>
+        <v>25.848368860948877</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184">
         <f t="shared" ca="1" si="4"/>
-        <v>2.108302074588003</v>
+        <v>1.354638533214227</v>
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="5"/>
-        <v>21.083020745880031</v>
+        <v>13.54638533214227</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185">
         <f t="shared" ca="1" si="4"/>
-        <v>3.74422919600008</v>
+        <v>3.1620714538109986</v>
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="5"/>
-        <v>37.442291960000802</v>
+        <v>31.620714538109986</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186">
         <f t="shared" ca="1" si="4"/>
-        <v>3.7583613638057267</v>
+        <v>3.8679373452417538</v>
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="5"/>
-        <v>37.583613638057265</v>
+        <v>38.679373452417536</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5542758948926654</v>
+        <v>1.7286934313828268</v>
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="5"/>
-        <v>35.542758948926654</v>
+        <v>17.286934313828269</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188">
         <f t="shared" ca="1" si="4"/>
-        <v>3.3903552878353795</v>
+        <v>3.4107537283761422</v>
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="5"/>
-        <v>33.903552878353793</v>
+        <v>34.107537283761424</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189">
         <f t="shared" ca="1" si="4"/>
-        <v>1.8002427475475968</v>
+        <v>2.6704273985880191</v>
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="5"/>
-        <v>18.002427475475969</v>
+        <v>26.704273985880192</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190">
         <f t="shared" ca="1" si="4"/>
-        <v>3.2972305032140659</v>
+        <v>1.8795877726509933</v>
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="5"/>
-        <v>32.97230503214066</v>
+        <v>18.795877726509932</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1673990929570954</v>
+        <v>3.7734384744003369</v>
       </c>
       <c r="B191">
         <f t="shared" ca="1" si="5"/>
-        <v>11.673990929570955</v>
+        <v>37.734384744003371</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7914177775495741</v>
+        <v>3.4108778838876552</v>
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="5"/>
-        <v>17.914177775495741</v>
+        <v>34.108778838876553</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193">
         <f t="shared" ca="1" si="4"/>
-        <v>1.3978744569552808</v>
+        <v>1.7357405190033086</v>
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="5"/>
-        <v>13.978744569552807</v>
+        <v>17.357405190033084</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194">
         <f t="shared" ca="1" si="4"/>
-        <v>2.394877743059233</v>
+        <v>3.794121983000371</v>
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="5"/>
-        <v>23.94877743059233</v>
+        <v>37.94121983000371</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195">
         <f t="shared" ref="A195:A249" ca="1" si="6">RAND() * (4 - 1) + 1</f>
-        <v>1.790307117738875</v>
+        <v>1.9276796465194561</v>
       </c>
       <c r="B195">
-        <f t="shared" ref="B195:B251" ca="1" si="7">A195*10</f>
-        <v>17.90307117738875</v>
+        <f t="shared" ref="B195:B249" ca="1" si="7">A195*10</f>
+        <v>19.276796465194561</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196">
         <f t="shared" ca="1" si="6"/>
-        <v>1.8152112902026207</v>
+        <v>1.5393145880763608</v>
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="7"/>
-        <v>18.152112902026207</v>
+        <v>15.393145880763608</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0393636607021985</v>
+        <v>2.7006936177682594</v>
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="7"/>
-        <v>10.393636607021985</v>
+        <v>27.006936177682594</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198">
         <f t="shared" ca="1" si="6"/>
-        <v>3.011082279085131</v>
+        <v>1.6723526520006027</v>
       </c>
       <c r="B198">
-        <f t="shared" ca="1" si="7"/>
-        <v>30.110822790851309</v>
+        <f ca="1">A198*5</f>
+        <v>8.3617632600030127</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199">
         <f t="shared" ca="1" si="6"/>
-        <v>3.6872885730342624</v>
+        <v>3.9848977268489811</v>
       </c>
       <c r="B199">
-        <f t="shared" ca="1" si="7"/>
-        <v>36.872885730342624</v>
+        <f t="shared" ref="B199:B238" ca="1" si="8">A199*5</f>
+        <v>19.924488634244906</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200">
         <f t="shared" ca="1" si="6"/>
-        <v>3.6636666800352944</v>
+        <v>2.5503653179352366</v>
       </c>
       <c r="B200">
-        <f t="shared" ca="1" si="7"/>
-        <v>36.636666800352941</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>12.751826589676183</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201">
         <f t="shared" ca="1" si="6"/>
-        <v>1.7763006268801989</v>
+        <v>3.775936136177342</v>
       </c>
       <c r="B201">
-        <f t="shared" ca="1" si="7"/>
-        <v>17.763006268801988</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>18.879680680886711</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202">
         <f t="shared" ca="1" si="6"/>
-        <v>2.094774852630604</v>
+        <v>1.7438558777293336</v>
       </c>
       <c r="B202">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.947748526306039</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.7192793886466688</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203">
         <f t="shared" ca="1" si="6"/>
-        <v>3.0385061737866641</v>
+        <v>3.2546333020932741</v>
       </c>
       <c r="B203">
-        <f t="shared" ca="1" si="7"/>
-        <v>30.385061737866643</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>16.273166510466371</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0784520511683136</v>
+        <v>2.1175657448247867</v>
       </c>
       <c r="B204">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.784520511683134</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>10.587828724123934</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205">
         <f t="shared" ca="1" si="6"/>
-        <v>3.8046720323356973</v>
+        <v>2.9540504378822483</v>
       </c>
       <c r="B205">
-        <f t="shared" ca="1" si="7"/>
-        <v>38.046720323356972</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>14.770252189411242</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206">
         <f t="shared" ca="1" si="6"/>
-        <v>1.361493988753844</v>
+        <v>1.1191223773470502</v>
       </c>
       <c r="B206">
-        <f t="shared" ca="1" si="7"/>
-        <v>13.614939887538441</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5.5956118867352513</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207">
         <f t="shared" ca="1" si="6"/>
-        <v>3.8640963353749109</v>
+        <v>1.2264807294819349</v>
       </c>
       <c r="B207">
-        <f t="shared" ca="1" si="7"/>
-        <v>38.640963353749108</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>6.1324036474096744</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4822853461163099</v>
+        <v>2.9663431879956792</v>
       </c>
       <c r="B208">
-        <f t="shared" ca="1" si="7"/>
-        <v>34.822853461163099</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>14.831715939978396</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209">
         <f t="shared" ca="1" si="6"/>
-        <v>2.8155412097813222</v>
+        <v>3.0165644161717933</v>
       </c>
       <c r="B209">
-        <f t="shared" ca="1" si="7"/>
-        <v>28.155412097813223</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>15.082822080858966</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210">
         <f t="shared" ca="1" si="6"/>
-        <v>3.669362165822037</v>
+        <v>3.7180013152795492</v>
       </c>
       <c r="B210">
-        <f t="shared" ca="1" si="7"/>
-        <v>36.693621658220373</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>18.590006576397748</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0179353417983705</v>
+        <v>2.6419737237481318</v>
       </c>
       <c r="B211">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.179353417983705</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>13.209868618740659</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212">
         <f t="shared" ca="1" si="6"/>
-        <v>3.2660837984001141</v>
+        <v>3.8934781342155573</v>
       </c>
       <c r="B212">
-        <f t="shared" ca="1" si="7"/>
-        <v>32.660837984001141</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>19.467390671077787</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7998789289784551</v>
+        <v>1.8902631337878055</v>
       </c>
       <c r="B213">
-        <f t="shared" ca="1" si="7"/>
-        <v>27.998789289784551</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>9.4513156689390279</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214">
         <f t="shared" ca="1" si="6"/>
-        <v>3.516364302563038</v>
+        <v>1.1785603524094084</v>
       </c>
       <c r="B214">
-        <f t="shared" ca="1" si="7"/>
-        <v>35.163643025630378</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5.8928017620470419</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215">
         <f t="shared" ca="1" si="6"/>
-        <v>2.4487833848239342</v>
+        <v>2.8375934187126672</v>
       </c>
       <c r="B215">
-        <f t="shared" ca="1" si="7"/>
-        <v>24.48783384823934</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>14.187967093563337</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0097794704075373</v>
+        <v>3.4895883201095246</v>
       </c>
       <c r="B216">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.097794704075373</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>17.447941600547622</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217">
         <f t="shared" ca="1" si="6"/>
-        <v>2.8864754421456702</v>
+        <v>2.7565676709654072</v>
       </c>
       <c r="B217">
-        <f t="shared" ca="1" si="7"/>
-        <v>28.864754421456702</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>13.782838354827035</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4671319404091925</v>
+        <v>3.0339405902604804</v>
       </c>
       <c r="B218">
-        <f t="shared" ca="1" si="7"/>
-        <v>34.671319404091925</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>15.169702951302401</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219">
         <f t="shared" ca="1" si="6"/>
-        <v>2.3911738278991344</v>
+        <v>1.4312003914179603</v>
       </c>
       <c r="B219">
-        <f t="shared" ca="1" si="7"/>
-        <v>23.911738278991344</v>
+        <f ca="1">A219*5</f>
+        <v>7.156001957089801</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3640502695378727</v>
+        <v>2.7422762882827167</v>
       </c>
       <c r="B220">
-        <f t="shared" ca="1" si="7"/>
-        <v>33.640502695378729</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>13.711381441413584</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221">
         <f t="shared" ca="1" si="6"/>
-        <v>1.2749925486436817</v>
+        <v>1.8874382272734773</v>
       </c>
       <c r="B221">
-        <f t="shared" ca="1" si="7"/>
-        <v>12.749925486436817</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>9.437191136367387</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222">
         <f t="shared" ca="1" si="6"/>
-        <v>3.1573341742617118</v>
+        <v>1.4633522242421051</v>
       </c>
       <c r="B222">
-        <f t="shared" ca="1" si="7"/>
-        <v>31.573341742617117</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>7.3167611212105257</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223">
         <f t="shared" ca="1" si="6"/>
-        <v>2.9299344073615323</v>
+        <v>1.3730276391218255</v>
       </c>
       <c r="B223">
-        <f t="shared" ca="1" si="7"/>
-        <v>29.299344073615323</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>6.8651381956091271</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224">
         <f t="shared" ca="1" si="6"/>
-        <v>2.9788724221582195</v>
+        <v>1.6646281747474001</v>
       </c>
       <c r="B224">
-        <f t="shared" ca="1" si="7"/>
-        <v>29.788724221582193</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.3231408737369996</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225">
         <f t="shared" ca="1" si="6"/>
-        <v>2.3190714662515148</v>
+        <v>1.666611333944229</v>
       </c>
       <c r="B225">
-        <f t="shared" ca="1" si="7"/>
-        <v>23.190714662515148</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.3330566697211452</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226">
         <f t="shared" ca="1" si="6"/>
-        <v>2.4469307986365259</v>
+        <v>3.2415477699596287</v>
       </c>
       <c r="B226">
-        <f t="shared" ca="1" si="7"/>
-        <v>24.469307986365259</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>16.207738849798144</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227">
         <f t="shared" ca="1" si="6"/>
-        <v>3.1724610335170764</v>
+        <v>2.327491104456525</v>
       </c>
       <c r="B227">
-        <f t="shared" ca="1" si="7"/>
-        <v>31.724610335170766</v>
+        <f ca="1">A227*5</f>
+        <v>11.637455522282625</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228">
         <f t="shared" ca="1" si="6"/>
-        <v>3.8859559270248223</v>
+        <v>3.1253475718678079</v>
       </c>
       <c r="B228">
-        <f t="shared" ca="1" si="7"/>
-        <v>38.859559270248226</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>15.626737859339039</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0105463932284451</v>
+        <v>1.5325140836055668</v>
       </c>
       <c r="B229">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.105463932284451</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>7.6625704180278342</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1286147381787679</v>
+        <v>2.5501901170835195</v>
       </c>
       <c r="B230">
-        <f t="shared" ca="1" si="7"/>
-        <v>11.286147381787679</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>12.750950585417598</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231">
         <f t="shared" ca="1" si="6"/>
-        <v>1.257244650048523</v>
+        <v>1.209652993062889</v>
       </c>
       <c r="B231">
-        <f t="shared" ca="1" si="7"/>
-        <v>12.572446500485231</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>6.0482649653144449</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232">
         <f t="shared" ca="1" si="6"/>
-        <v>3.0420841307871003</v>
+        <v>3.2904743467753907</v>
       </c>
       <c r="B232">
-        <f t="shared" ca="1" si="7"/>
-        <v>30.420841307871001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>16.452371733876955</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233">
         <f t="shared" ca="1" si="6"/>
-        <v>3.5647149255707213</v>
+        <v>3.2048681626525903</v>
       </c>
       <c r="B233">
-        <f t="shared" ca="1" si="7"/>
-        <v>35.647149255707212</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>16.024340813262953</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234">
         <f t="shared" ca="1" si="6"/>
-        <v>3.7154178577925525</v>
+        <v>3.1536104324328607</v>
       </c>
       <c r="B234">
-        <f t="shared" ca="1" si="7"/>
-        <v>37.154178577925528</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>15.768052162164302</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235">
         <f t="shared" ca="1" si="6"/>
-        <v>1.91031064357629</v>
+        <v>2.2280895279901838</v>
       </c>
       <c r="B235">
-        <f t="shared" ca="1" si="7"/>
-        <v>19.1031064357629</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>11.140447639950919</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236">
         <f t="shared" ca="1" si="6"/>
-        <v>3.9581205206097421</v>
+        <v>1.4959391976722887</v>
       </c>
       <c r="B236">
-        <f t="shared" ca="1" si="7"/>
-        <v>39.581205206097422</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>7.4796959883614438</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237">
         <f t="shared" ca="1" si="6"/>
-        <v>1.3819633856950926</v>
+        <v>2.0386136325426376</v>
       </c>
       <c r="B237">
-        <f t="shared" ca="1" si="7"/>
-        <v>13.819633856950926</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>10.193068162713189</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238">
         <f t="shared" ca="1" si="6"/>
-        <v>2.6784010151114681</v>
+        <v>2.937300408893603</v>
       </c>
       <c r="B238">
-        <f t="shared" ca="1" si="7"/>
-        <v>26.784010151114682</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>14.686502044468014</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239">
         <f t="shared" ca="1" si="6"/>
-        <v>2.119308421645596</v>
+        <v>3.4709360855745719</v>
       </c>
       <c r="B239">
         <f t="shared" ca="1" si="7"/>
-        <v>21.193084216455958</v>
+        <v>34.709360855745722</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240">
         <f t="shared" ca="1" si="6"/>
-        <v>1.9959162865605384</v>
+        <v>2.0600738583044853</v>
       </c>
       <c r="B240">
         <f t="shared" ca="1" si="7"/>
-        <v>19.959162865605386</v>
+        <v>20.600738583044851</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0202118500933168</v>
+        <v>2.165284044429943</v>
       </c>
       <c r="B241">
         <f t="shared" ca="1" si="7"/>
-        <v>20.202118500933167</v>
+        <v>21.652840444299429</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242">
         <f t="shared" ca="1" si="6"/>
-        <v>3.5719775319145977</v>
+        <v>3.046081142212135</v>
       </c>
       <c r="B242">
         <f t="shared" ca="1" si="7"/>
-        <v>35.719775319145974</v>
+        <v>30.460811422121349</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243">
         <f t="shared" ca="1" si="6"/>
-        <v>2.5313167632783502</v>
+        <v>2.4502967289592719</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244">
         <f t="shared" ca="1" si="6"/>
-        <v>2.2178911809103274</v>
+        <v>3.0371044579235251</v>
       </c>
       <c r="B244">
         <f t="shared" ca="1" si="7"/>
-        <v>22.178911809103276</v>
+        <v>30.371044579235253</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245">
         <f t="shared" ca="1" si="6"/>
-        <v>3.5359709295569259</v>
+        <v>3.4454490298109679</v>
       </c>
       <c r="B245">
         <f t="shared" ca="1" si="7"/>
-        <v>35.35970929556926</v>
+        <v>34.454490298109675</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3243723015843245</v>
+        <v>2.0036820325703628</v>
       </c>
       <c r="B246">
         <f t="shared" ca="1" si="7"/>
-        <v>33.243723015843244</v>
+        <v>20.03682032570363</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247">
         <f t="shared" ca="1" si="6"/>
-        <v>3.8978980163381585</v>
+        <v>1.8925473724514426</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248">
         <f t="shared" ca="1" si="6"/>
-        <v>3.6134059882293093</v>
+        <v>3.7861668441653409</v>
       </c>
       <c r="B248">
         <f t="shared" ca="1" si="7"/>
-        <v>36.134059882293094</v>
+        <v>37.861668441653407</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7643514668965365</v>
+        <v>1.1271480769081892</v>
       </c>
       <c r="B249">
         <f t="shared" ca="1" si="7"/>
-        <v>27.643514668965366</v>
+        <v>11.271480769081892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>